<commit_message>
somewhy obtaining std and mean of monomer slicing makes problems in dataframe
</commit_message>
<xml_diff>
--- a/add_data/130721raw_monomer_sampling.xlsx
+++ b/add_data/130721raw_monomer_sampling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amityu\DataspellProjects\gel_sheets\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71EFA11D-DAFF-4F67-89C5-8614C3303BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68713427-8D4D-40DB-B410-3AB2C6C41D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C26667C-A685-4EB0-8425-5B3C50599133}"/>
   </bookViews>
@@ -44,19 +44,19 @@
     <t>i_start</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>j_start</t>
   </si>
   <si>
     <t>i_gap</t>
   </si>
   <si>
-    <t>j_jap</t>
+    <t>z_gap</t>
   </si>
   <si>
-    <t>z_gap</t>
+    <t>z_start</t>
+  </si>
+  <si>
+    <t>j_gap</t>
   </si>
 </sst>
 </file>
@@ -408,38 +408,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083E994A-22EC-4F0F-9A92-2E91951B8C43}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:G63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:F126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -485,7 +485,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -508,7 +508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -531,7 +531,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -554,7 +554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -577,7 +577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -600,7 +600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -623,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -646,7 +646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -669,7 +669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -692,7 +692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -715,7 +715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -738,7 +738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -761,7 +761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -784,7 +784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -807,7 +807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -830,7 +830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -853,7 +853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -876,7 +876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -899,7 +899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -922,7 +922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -945,7 +945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -968,7 +968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -991,7 +991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1863,311 +1863,6 @@
       </c>
       <c r="G63">
         <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A64">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A76">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A82">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A83">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A84">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A85">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A86">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A88">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A89">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A90">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A91">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A92">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A93">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A94">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A95">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A96">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A97">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A98">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A99">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A100">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A101">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A102">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A103">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A104">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A105">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A106">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A107">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A108">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A109">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A110">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A111">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A112">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A113">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A114">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A115">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A116">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A117">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A118">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A119">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A120">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A121">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A122">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A123">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A124">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
monomer bg slices where filled for 130721raw
</commit_message>
<xml_diff>
--- a/add_data/130721raw_monomer_sampling.xlsx
+++ b/add_data/130721raw_monomer_sampling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amityu\DataspellProjects\gel_sheets\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68713427-8D4D-40DB-B410-3AB2C6C41D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0312BCA4-7E12-4315-8394-F98A7D2E5B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C26667C-A685-4EB0-8425-5B3C50599133}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0C26667C-A685-4EB0-8425-5B3C50599133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>t</t>
   </si>
   <si>
-    <t>i_start</t>
-  </si>
-  <si>
     <t>j_start</t>
-  </si>
-  <si>
-    <t>i_gap</t>
   </si>
   <si>
     <t>z_gap</t>
@@ -408,38 +402,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083E994A-22EC-4F0F-9A92-2E91951B8C43}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:F126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -450,180 +438,132 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
       <c r="D3">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E5">
         <v>20</v>
       </c>
-      <c r="F5">
-        <v>490</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="F6">
-        <v>490</v>
-      </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
-      <c r="F7">
-        <v>490</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
-      <c r="F8">
-        <v>490</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E9">
         <v>20</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -634,19 +574,13 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E10">
         <v>20</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -657,19 +591,13 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E11">
         <v>20</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -680,19 +608,13 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E12">
         <v>20</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -703,19 +625,13 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E13">
         <v>20</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -726,19 +642,13 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E14">
         <v>20</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -749,19 +659,13 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E15">
         <v>20</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -772,19 +676,13 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E16">
         <v>20</v>
       </c>
-      <c r="F16">
-        <v>100</v>
-      </c>
-      <c r="G16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -795,19 +693,13 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E17">
         <v>20</v>
       </c>
-      <c r="F17">
-        <v>110</v>
-      </c>
-      <c r="G17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -818,19 +710,13 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="E18">
         <v>20</v>
       </c>
-      <c r="F18">
-        <v>110</v>
-      </c>
-      <c r="G18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -841,410 +727,302 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>20</v>
       </c>
-      <c r="F19">
-        <v>110</v>
-      </c>
-      <c r="G19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E20">
         <v>20</v>
       </c>
-      <c r="F20">
-        <v>110</v>
-      </c>
-      <c r="G20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
-      <c r="F21">
-        <v>280</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
-      <c r="F22">
-        <v>280</v>
-      </c>
-      <c r="G22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E23">
         <v>20</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
       <c r="D24">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E24">
         <v>20</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
       <c r="D25">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E25">
         <v>20</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="D26">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E26">
         <v>20</v>
       </c>
-      <c r="F26">
-        <v>50</v>
-      </c>
-      <c r="G26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C27">
         <v>10</v>
       </c>
       <c r="D27">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E27">
         <v>20</v>
       </c>
-      <c r="F27">
-        <v>50</v>
-      </c>
-      <c r="G27">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
       <c r="D28">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E28">
         <v>20</v>
       </c>
-      <c r="F28">
-        <v>50</v>
-      </c>
-      <c r="G28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
       <c r="D29">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E29">
         <v>20</v>
       </c>
-      <c r="F29">
-        <v>50</v>
-      </c>
-      <c r="G29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C30">
         <v>10</v>
       </c>
       <c r="D30">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E30">
         <v>20</v>
       </c>
-      <c r="F30">
-        <v>50</v>
-      </c>
-      <c r="G30">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C31">
         <v>10</v>
       </c>
       <c r="D31">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E31">
         <v>20</v>
       </c>
-      <c r="F31">
-        <v>50</v>
-      </c>
-      <c r="G31">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="D32">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E32">
         <v>20</v>
       </c>
-      <c r="F32">
-        <v>50</v>
-      </c>
-      <c r="G32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
       <c r="D33">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E33">
         <v>20</v>
       </c>
-      <c r="F33">
-        <v>50</v>
-      </c>
-      <c r="G33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C34">
         <v>10</v>
       </c>
       <c r="D34">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E34">
         <v>20</v>
       </c>
-      <c r="F34">
-        <v>50</v>
-      </c>
-      <c r="G34">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C35">
         <v>10</v>
       </c>
       <c r="D35">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E35">
         <v>20</v>
       </c>
-      <c r="F35">
-        <v>50</v>
-      </c>
-      <c r="G35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C36">
         <v>10</v>
       </c>
       <c r="D36">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E36">
         <v>20</v>
       </c>
-      <c r="F36">
-        <v>50</v>
-      </c>
-      <c r="G36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1255,613 +1033,451 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E37">
         <v>20</v>
       </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="D38">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E38">
         <v>20</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C39">
         <v>10</v>
       </c>
       <c r="D39">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E39">
         <v>20</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C40">
         <v>10</v>
       </c>
       <c r="D40">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E40">
         <v>20</v>
       </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C41">
         <v>10</v>
       </c>
       <c r="D41">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E41">
         <v>20</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C42">
         <v>10</v>
       </c>
       <c r="D42">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E42">
         <v>20</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C43">
         <v>10</v>
       </c>
       <c r="D43">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E43">
         <v>20</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C44">
         <v>10</v>
       </c>
       <c r="D44">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E44">
         <v>20</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C45">
         <v>10</v>
       </c>
       <c r="D45">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E45">
         <v>20</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C46">
         <v>10</v>
       </c>
       <c r="D46">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E46">
         <v>20</v>
       </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C47">
         <v>10</v>
       </c>
       <c r="D47">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E47">
         <v>20</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>10</v>
       </c>
       <c r="D48">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E48">
         <v>20</v>
       </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C49">
         <v>10</v>
       </c>
       <c r="D49">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E49">
         <v>20</v>
       </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C50">
         <v>10</v>
       </c>
       <c r="D50">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E50">
         <v>20</v>
       </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C51">
         <v>10</v>
       </c>
       <c r="D51">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E51">
         <v>20</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C52">
         <v>10</v>
       </c>
       <c r="D52">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E52">
         <v>20</v>
       </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C53">
         <v>10</v>
       </c>
       <c r="D53">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E53">
         <v>20</v>
       </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C54">
         <v>10</v>
       </c>
       <c r="D54">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E54">
         <v>20</v>
       </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C55">
         <v>10</v>
       </c>
       <c r="D55">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E55">
         <v>20</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C56">
         <v>10</v>
       </c>
       <c r="D56">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E56">
         <v>20</v>
       </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C57">
         <v>10</v>
       </c>
       <c r="D57">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E57">
         <v>20</v>
       </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C58">
         <v>10</v>
       </c>
       <c r="D58">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E58">
         <v>20</v>
       </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C59">
         <v>10</v>
       </c>
       <c r="D59">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E59">
         <v>20</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C60">
         <v>10</v>
       </c>
       <c r="D60">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E60">
         <v>20</v>
       </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C61">
         <v>10</v>
       </c>
       <c r="D61">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E61">
         <v>20</v>
       </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C62">
         <v>10</v>
       </c>
       <c r="D62">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E62">
         <v>20</v>
       </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-      <c r="G62">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C63">
         <v>10</v>
       </c>
       <c r="D63">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="E63">
-        <v>20</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
After gefen advice, trying otsu, vs monomer std to thresh and view
</commit_message>
<xml_diff>
--- a/add_data/130721raw_monomer_sampling.xlsx
+++ b/add_data/130721raw_monomer_sampling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amityu\DataspellProjects\gel_sheets\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0312BCA4-7E12-4315-8394-F98A7D2E5B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3504D89-EAF0-4B61-9766-553C9FD5CF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0C26667C-A685-4EB0-8425-5B3C50599133}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -534,10 +534,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>300</v>
@@ -656,7 +656,7 @@
         <v>70</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>300</v>
@@ -673,7 +673,7 @@
         <v>70</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>300</v>
@@ -741,7 +741,7 @@
         <v>80</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>500</v>
@@ -789,7 +789,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -806,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -823,7 +823,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -840,7 +840,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -857,7 +857,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -874,7 +874,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -891,7 +891,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -908,7 +908,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -925,7 +925,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -942,7 +942,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -959,7 +959,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -976,7 +976,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -993,7 +993,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -1010,7 +1010,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -1027,7 +1027,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -1044,7 +1044,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1061,7 +1061,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -1078,7 +1078,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -1095,7 +1095,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C41">
         <v>10</v>
@@ -1112,7 +1112,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C42">
         <v>10</v>

</xml_diff>